<commit_message>
evaluate rki_children use case without scas variables using a p leave out cv approach
</commit_message>
<xml_diff>
--- a/results/tables/approaches/sorted_users/raw_results.xlsx
+++ b/results/tables/approaches/sorted_users/raw_results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joa24jm\Documents\UsAs\results\tables\approaches\sorted_users\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johannesallgaier/PycharmProjects/UsAs/results/tables/approaches/sorted_users/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{5509AEAE-1A72-4F4E-9163-06A986786BB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1D6A795-A089-B243-A492-5091F350ECCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="raw_results" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,25 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">raw_results!$A$2:$V$10</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">Sheet1!$A$1:$L$32</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="49">
   <si>
     <t>cc_f1</t>
   </si>
@@ -141,16 +154,7 @@
     <t>Score</t>
   </si>
   <si>
-    <t>F1 Test</t>
-  </si>
-  <si>
-    <t>F1 Validation</t>
-  </si>
-  <si>
     <t>Performance Drop</t>
-  </si>
-  <si>
-    <t>Std Validation</t>
   </si>
   <si>
     <t>User-Level</t>
@@ -197,8 +201,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="20" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -796,27 +800,6 @@
   <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -832,7 +815,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="18" fillId="0" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -863,6 +846,9 @@
     <xf numFmtId="10" fontId="19" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -872,8 +858,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -1025,6 +1029,2008 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>610696</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="595804" cy="736600"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2" name="TextBox 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{44AB3C05-0209-98AD-0391-54C9E0826E07}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2960196" y="571500"/>
+              <a:ext cx="595804" cy="736600"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:noAutofit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="r"/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="right"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:r>
+                      <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>𝜎</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>(</m:t>
+                    </m:r>
+                    <m:sSubSup>
+                      <m:sSubSupPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubSupPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑓</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>1</m:t>
+                        </m:r>
+                      </m:sub>
+                      <m:sup>
+                        <m:r>
+                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑡𝑟𝑎𝑖𝑛</m:t>
+                        </m:r>
+                      </m:sup>
+                    </m:sSubSup>
+                    <m:r>
+                      <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>)</m:t>
+                    </m:r>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+            <a:p>
+              <a:pPr algn="r"/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="right"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:sSubSup>
+                      <m:sSubSupPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubSupPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑓</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>1</m:t>
+                        </m:r>
+                      </m:sub>
+                      <m:sup>
+                        <m:r>
+                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑡𝑟𝑎𝑖𝑛</m:t>
+                        </m:r>
+                      </m:sup>
+                    </m:sSubSup>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+            <a:p>
+              <a:pPr algn="r"/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="right"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:sSubSup>
+                      <m:sSubSupPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubSupPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑓</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>1</m:t>
+                        </m:r>
+                      </m:sub>
+                      <m:sup>
+                        <m:r>
+                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑡𝑒𝑠𝑡</m:t>
+                        </m:r>
+                      </m:sup>
+                    </m:sSubSup>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2" name="TextBox 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{44AB3C05-0209-98AD-0391-54C9E0826E07}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2960196" y="571500"/>
+              <a:ext cx="595804" cy="736600"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:noAutofit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="r"/>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝜎(𝑓_1^𝑡𝑟𝑎𝑖𝑛)</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+            <a:p>
+              <a:pPr algn="r"/>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑓_1^𝑡𝑟𝑎𝑖𝑛</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+            <a:p>
+              <a:pPr algn="r"/>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑓_1^𝑡𝑒𝑠𝑡</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>610696</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="595804" cy="749300"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="4" name="TextBox 3">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FDBEBDF6-C827-0449-9245-AC66D60F02C6}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2960196" y="1308100"/>
+              <a:ext cx="595804" cy="749300"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:noAutofit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="r"/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="right"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:r>
+                      <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>𝜎</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>(</m:t>
+                    </m:r>
+                    <m:sSubSup>
+                      <m:sSubSupPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubSupPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑓</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>1</m:t>
+                        </m:r>
+                      </m:sub>
+                      <m:sup>
+                        <m:r>
+                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑡𝑟𝑎𝑖𝑛</m:t>
+                        </m:r>
+                      </m:sup>
+                    </m:sSubSup>
+                    <m:r>
+                      <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>)</m:t>
+                    </m:r>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+            <a:p>
+              <a:pPr algn="r"/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="right"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:sSubSup>
+                      <m:sSubSupPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubSupPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑓</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>1</m:t>
+                        </m:r>
+                      </m:sub>
+                      <m:sup>
+                        <m:r>
+                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑡𝑟𝑎𝑖𝑛</m:t>
+                        </m:r>
+                      </m:sup>
+                    </m:sSubSup>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+            <a:p>
+              <a:pPr algn="r"/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="right"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:sSubSup>
+                      <m:sSubSupPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubSupPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑓</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>1</m:t>
+                        </m:r>
+                      </m:sub>
+                      <m:sup>
+                        <m:r>
+                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑡𝑒𝑠𝑡</m:t>
+                        </m:r>
+                      </m:sup>
+                    </m:sSubSup>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="4" name="TextBox 3">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FDBEBDF6-C827-0449-9245-AC66D60F02C6}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2960196" y="1308100"/>
+              <a:ext cx="595804" cy="749300"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:noAutofit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="r"/>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝜎(𝑓_1^𝑡𝑟𝑎𝑖𝑛)</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+            <a:p>
+              <a:pPr algn="r"/>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑓_1^𝑡𝑟𝑎𝑖𝑛</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+            <a:p>
+              <a:pPr algn="r"/>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑓_1^𝑡𝑒𝑠𝑡</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>610696</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="595804" cy="749300"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="5" name="TextBox 4">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{56C0118C-F2FC-6945-BA0E-F72BA1D5F385}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2960196" y="2057400"/>
+              <a:ext cx="595804" cy="749300"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:noAutofit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="r"/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="right"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:r>
+                      <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>𝜎</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>(</m:t>
+                    </m:r>
+                    <m:sSubSup>
+                      <m:sSubSupPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubSupPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑓</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>1</m:t>
+                        </m:r>
+                      </m:sub>
+                      <m:sup>
+                        <m:r>
+                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑡𝑟𝑎𝑖𝑛</m:t>
+                        </m:r>
+                      </m:sup>
+                    </m:sSubSup>
+                    <m:r>
+                      <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>)</m:t>
+                    </m:r>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+            <a:p>
+              <a:pPr algn="r"/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="right"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:sSubSup>
+                      <m:sSubSupPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubSupPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑓</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>1</m:t>
+                        </m:r>
+                      </m:sub>
+                      <m:sup>
+                        <m:r>
+                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑡𝑟𝑎𝑖𝑛</m:t>
+                        </m:r>
+                      </m:sup>
+                    </m:sSubSup>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+            <a:p>
+              <a:pPr algn="r"/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="right"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:sSubSup>
+                      <m:sSubSupPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubSupPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑓</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>1</m:t>
+                        </m:r>
+                      </m:sub>
+                      <m:sup>
+                        <m:r>
+                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑡𝑒𝑠𝑡</m:t>
+                        </m:r>
+                      </m:sup>
+                    </m:sSubSup>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="5" name="TextBox 4">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{56C0118C-F2FC-6945-BA0E-F72BA1D5F385}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2960196" y="2057400"/>
+              <a:ext cx="595804" cy="749300"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:noAutofit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="r"/>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝜎(𝑓_1^𝑡𝑟𝑎𝑖𝑛)</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+            <a:p>
+              <a:pPr algn="r"/>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑓_1^𝑡𝑟𝑎𝑖𝑛</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+            <a:p>
+              <a:pPr algn="r"/>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑓_1^𝑡𝑒𝑠𝑡</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>610696</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="595804" cy="749300"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="6" name="TextBox 5">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{14E08C44-1DAA-A246-B804-920107FA5B10}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2960196" y="2806700"/>
+              <a:ext cx="595804" cy="749300"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:noAutofit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="r"/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="right"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:r>
+                      <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>𝜎</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>(</m:t>
+                    </m:r>
+                    <m:sSubSup>
+                      <m:sSubSupPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubSupPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑓</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>1</m:t>
+                        </m:r>
+                      </m:sub>
+                      <m:sup>
+                        <m:r>
+                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑡𝑟𝑎𝑖𝑛</m:t>
+                        </m:r>
+                      </m:sup>
+                    </m:sSubSup>
+                    <m:r>
+                      <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>)</m:t>
+                    </m:r>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+            <a:p>
+              <a:pPr algn="r"/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="right"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:sSubSup>
+                      <m:sSubSupPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubSupPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑓</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>1</m:t>
+                        </m:r>
+                      </m:sub>
+                      <m:sup>
+                        <m:r>
+                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑡𝑟𝑎𝑖𝑛</m:t>
+                        </m:r>
+                      </m:sup>
+                    </m:sSubSup>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+            <a:p>
+              <a:pPr algn="r"/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="right"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:sSubSup>
+                      <m:sSubSupPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubSupPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑓</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>1</m:t>
+                        </m:r>
+                      </m:sub>
+                      <m:sup>
+                        <m:r>
+                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑡𝑒𝑠𝑡</m:t>
+                        </m:r>
+                      </m:sup>
+                    </m:sSubSup>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="6" name="TextBox 5">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{14E08C44-1DAA-A246-B804-920107FA5B10}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2960196" y="2806700"/>
+              <a:ext cx="595804" cy="749300"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:noAutofit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="r"/>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝜎(𝑓_1^𝑡𝑟𝑎𝑖𝑛)</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+            <a:p>
+              <a:pPr algn="r"/>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑓_1^𝑡𝑟𝑎𝑖𝑛</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+            <a:p>
+              <a:pPr algn="r"/>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑓_1^𝑡𝑒𝑠𝑡</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>610696</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="595804" cy="749300"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="7" name="TextBox 6">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8DF7C43C-8583-B54A-A3A3-9142A026E566}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2960196" y="3556000"/>
+              <a:ext cx="595804" cy="749300"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:noAutofit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="r"/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="right"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:r>
+                      <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>𝜎</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>(</m:t>
+                    </m:r>
+                    <m:sSubSup>
+                      <m:sSubSupPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubSupPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑓</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>1</m:t>
+                        </m:r>
+                      </m:sub>
+                      <m:sup>
+                        <m:r>
+                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑡𝑟𝑎𝑖𝑛</m:t>
+                        </m:r>
+                      </m:sup>
+                    </m:sSubSup>
+                    <m:r>
+                      <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>)</m:t>
+                    </m:r>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+            <a:p>
+              <a:pPr algn="r"/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="right"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:sSubSup>
+                      <m:sSubSupPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubSupPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑓</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>1</m:t>
+                        </m:r>
+                      </m:sub>
+                      <m:sup>
+                        <m:r>
+                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑡𝑟𝑎𝑖𝑛</m:t>
+                        </m:r>
+                      </m:sup>
+                    </m:sSubSup>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+            <a:p>
+              <a:pPr algn="r"/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="right"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:sSubSup>
+                      <m:sSubSupPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubSupPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑓</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>1</m:t>
+                        </m:r>
+                      </m:sub>
+                      <m:sup>
+                        <m:r>
+                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑡𝑒𝑠𝑡</m:t>
+                        </m:r>
+                      </m:sup>
+                    </m:sSubSup>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="7" name="TextBox 6">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8DF7C43C-8583-B54A-A3A3-9142A026E566}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2960196" y="3556000"/>
+              <a:ext cx="595804" cy="749300"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:noAutofit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="r"/>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝜎(𝑓_1^𝑡𝑟𝑎𝑖𝑛)</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+            <a:p>
+              <a:pPr algn="r"/>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑓_1^𝑡𝑟𝑎𝑖𝑛</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+            <a:p>
+              <a:pPr algn="r"/>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑓_1^𝑡𝑒𝑠𝑡</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>610696</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="595804" cy="723900"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="8" name="TextBox 7">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AC277BAF-0E27-7B4B-AAFC-553CF1EA24EA}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2960196" y="4305300"/>
+              <a:ext cx="595804" cy="723900"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:noAutofit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="r"/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="right"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:r>
+                      <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>𝜎</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>(</m:t>
+                    </m:r>
+                    <m:sSubSup>
+                      <m:sSubSupPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubSupPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑓</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>1</m:t>
+                        </m:r>
+                      </m:sub>
+                      <m:sup>
+                        <m:r>
+                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑡𝑟𝑎𝑖𝑛</m:t>
+                        </m:r>
+                      </m:sup>
+                    </m:sSubSup>
+                    <m:r>
+                      <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>)</m:t>
+                    </m:r>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+            <a:p>
+              <a:pPr algn="r"/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="right"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:sSubSup>
+                      <m:sSubSupPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubSupPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑓</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>1</m:t>
+                        </m:r>
+                      </m:sub>
+                      <m:sup>
+                        <m:r>
+                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑡𝑟𝑎𝑖𝑛</m:t>
+                        </m:r>
+                      </m:sup>
+                    </m:sSubSup>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+            <a:p>
+              <a:pPr algn="r"/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="right"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:sSubSup>
+                      <m:sSubSupPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubSupPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑓</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>1</m:t>
+                        </m:r>
+                      </m:sub>
+                      <m:sup>
+                        <m:r>
+                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑡𝑒𝑠𝑡</m:t>
+                        </m:r>
+                      </m:sup>
+                    </m:sSubSup>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="8" name="TextBox 7">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AC277BAF-0E27-7B4B-AAFC-553CF1EA24EA}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2960196" y="4305300"/>
+              <a:ext cx="595804" cy="723900"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:noAutofit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="r"/>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝜎(𝑓_1^𝑡𝑟𝑎𝑖𝑛)</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+            <a:p>
+              <a:pPr algn="r"/>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑓_1^𝑡𝑟𝑎𝑖𝑛</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+            <a:p>
+              <a:pPr algn="r"/>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑓_1^𝑡𝑒𝑠𝑡</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>610696</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>184150</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="595804" cy="749300"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="9" name="TextBox 8">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{688DB725-6EFE-0D48-A0D2-29C83F3D513C}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2960196" y="5022850"/>
+              <a:ext cx="595804" cy="749300"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:noAutofit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="r"/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="right"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:r>
+                      <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>𝜎</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>(</m:t>
+                    </m:r>
+                    <m:sSubSup>
+                      <m:sSubSupPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubSupPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑓</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>1</m:t>
+                        </m:r>
+                      </m:sub>
+                      <m:sup>
+                        <m:r>
+                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑡𝑟𝑎𝑖𝑛</m:t>
+                        </m:r>
+                      </m:sup>
+                    </m:sSubSup>
+                    <m:r>
+                      <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>)</m:t>
+                    </m:r>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+            <a:p>
+              <a:pPr algn="r"/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="right"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:sSubSup>
+                      <m:sSubSupPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubSupPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑓</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>1</m:t>
+                        </m:r>
+                      </m:sub>
+                      <m:sup>
+                        <m:r>
+                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑡𝑟𝑎𝑖𝑛</m:t>
+                        </m:r>
+                      </m:sup>
+                    </m:sSubSup>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+            <a:p>
+              <a:pPr algn="r"/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="right"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:sSubSup>
+                      <m:sSubSupPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubSupPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑓</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>1</m:t>
+                        </m:r>
+                      </m:sub>
+                      <m:sup>
+                        <m:r>
+                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑡𝑒𝑠𝑡</m:t>
+                        </m:r>
+                      </m:sup>
+                    </m:sSubSup>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="9" name="TextBox 8">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{688DB725-6EFE-0D48-A0D2-29C83F3D513C}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2960196" y="5022850"/>
+              <a:ext cx="595804" cy="749300"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:noAutofit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="r"/>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝜎(𝑓_1^𝑡𝑟𝑎𝑖𝑛)</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+            <a:p>
+              <a:pPr algn="r"/>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑓_1^𝑡𝑟𝑎𝑖𝑛</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+            <a:p>
+              <a:pPr algn="r"/>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑓_1^𝑡𝑒𝑠𝑡</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1324,7 +3330,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:V10"/>
   <sheetViews>
@@ -1332,66 +3338,66 @@
       <selection activeCell="K33" sqref="K33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="12" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="12" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="14" max="15" width="12" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="17" max="18" width="12" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="20" max="21" width="12" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22">
       <c r="A1" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2" t="s">
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2" t="s">
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2" t="s">
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2" t="s">
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2" t="s">
+      <c r="O1" s="18"/>
+      <c r="P1" s="18"/>
+      <c r="Q1" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2" t="s">
+      <c r="R1" s="18"/>
+      <c r="S1" s="18"/>
+      <c r="T1" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2"/>
+      <c r="U1" s="18"/>
+      <c r="V1" s="18"/>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -1456,7 +3462,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" hidden="1">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -1503,7 +3509,7 @@
         <v>4.8722756023569999E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" hidden="1">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -1550,7 +3556,7 @@
         <v>5.4332817729540002E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" hidden="1">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -1597,7 +3603,7 @@
         <v>6.6029163881887003E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" hidden="1">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -1644,7 +3650,7 @@
         <v>1.07673662880334E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" s="1" customFormat="1">
       <c r="A7" s="1" t="s">
         <v>25</v>
       </c>
@@ -1712,7 +3718,7 @@
         <v>0.55812760815291595</v>
       </c>
     </row>
-    <row r="8" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" s="1" customFormat="1">
       <c r="A8" s="1" t="s">
         <v>26</v>
       </c>
@@ -1780,7 +3786,7 @@
         <v>0.58304667288122403</v>
       </c>
     </row>
-    <row r="9" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22" hidden="1">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -1821,7 +3827,7 @@
         <v>0.163149278499262</v>
       </c>
     </row>
-    <row r="10" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22" s="1" customFormat="1">
       <c r="A10" s="1" t="s">
         <v>28</v>
       </c>
@@ -1890,7 +3896,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:V10">
+  <autoFilter ref="A2:V10" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <filterColumn colId="3">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -1907,75 +3913,74 @@
     <mergeCell ref="Q1:S1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:J31"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="150" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="2" customWidth="1"/>
-    <col min="2" max="2" width="28.77734375" customWidth="1"/>
-    <col min="3" max="3" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.83203125" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="2.21875" customWidth="1"/>
+    <col min="7" max="7" width="2.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" ht="17.25" x14ac:dyDescent="0.35">
-      <c r="B2" s="6" t="s">
+    <row r="2" spans="2:10" ht="15">
+      <c r="B2" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="7" t="s">
+      <c r="C2" s="7"/>
+      <c r="D2" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" s="23"/>
+      <c r="F2" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H2" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+    </row>
+    <row r="3" spans="2:10" ht="16.5" customHeight="1" thickBot="1">
+      <c r="B3" s="28"/>
+      <c r="C3" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" ht="15" thickTop="1">
+      <c r="B4" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="E2" s="5"/>
-      <c r="F2" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-    </row>
-    <row r="3" spans="2:10" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="8"/>
-      <c r="C3" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="F3" s="18" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="2:10" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="28" t="s">
-        <v>45</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="D4" s="9">
+      <c r="C4" s="6"/>
+      <c r="D4" s="2">
         <v>1.42299652232106E-2</v>
       </c>
-      <c r="E4" s="10">
+      <c r="E4" s="3">
         <v>4.6939627280001797E-2</v>
       </c>
-      <c r="F4" s="19">
+      <c r="F4" s="12">
         <v>5.3796214513514001E-3</v>
       </c>
       <c r="H4" t="b">
@@ -1991,68 +3996,62 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B5" s="3"/>
-      <c r="C5" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="D5" s="22">
+    <row r="5" spans="2:10">
+      <c r="B5" s="25"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="15">
         <v>0.76804452183438199</v>
       </c>
-      <c r="E5" s="10">
+      <c r="E5" s="3">
         <v>0.72498310422866197</v>
       </c>
-      <c r="F5" s="19">
+      <c r="F5" s="12">
         <v>0.775698990359178</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B6" s="3"/>
-      <c r="C6" s="13" t="s">
+    <row r="6" spans="2:10">
+      <c r="B6" s="25"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="2">
+        <v>0.67536994924959404</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0.64601515307857804</v>
+      </c>
+      <c r="F6" s="12">
+        <v>0.67979512113552298</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" ht="15">
+      <c r="B7" s="26"/>
+      <c r="C7" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="D6" s="9">
-        <v>0.67536994924959404</v>
-      </c>
-      <c r="E6" s="10">
-        <v>0.64601515307857804</v>
-      </c>
-      <c r="F6" s="19">
-        <v>0.67979512113552298</v>
-      </c>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B7" s="4"/>
-      <c r="C7" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="D7" s="11">
+      <c r="D7" s="4">
         <f>D6-D5</f>
         <v>-9.2674572584787951E-2</v>
       </c>
-      <c r="E7" s="12">
+      <c r="E7" s="5">
         <f>E6-E5</f>
         <v>-7.8967951150083926E-2</v>
       </c>
-      <c r="F7" s="20">
+      <c r="F7" s="13">
         <f>F6-F5</f>
         <v>-9.5903869223655014E-2</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B8" s="25" t="s">
-        <v>46</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="D8" s="9">
+    <row r="8" spans="2:10">
+      <c r="B8" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="6"/>
+      <c r="D8" s="2">
         <v>4.9499215596577703E-2</v>
       </c>
-      <c r="E8" s="23">
+      <c r="E8" s="16">
         <v>3.58651735003667E-2</v>
       </c>
-      <c r="F8" s="19">
+      <c r="F8" s="12">
         <v>1.2902419742930099E-2</v>
       </c>
       <c r="H8" t="b">
@@ -2068,68 +4067,62 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B9" s="26"/>
-      <c r="C9" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="D9" s="22">
+    <row r="9" spans="2:10">
+      <c r="B9" s="20"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="15">
         <v>0.54731897033183097</v>
       </c>
-      <c r="E9" s="23">
+      <c r="E9" s="16">
         <v>0.51192225783675005</v>
       </c>
-      <c r="F9" s="19">
+      <c r="F9" s="12">
         <v>0.57465660291915399</v>
       </c>
     </row>
-    <row r="10" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="26"/>
-      <c r="C10" s="13" t="s">
+    <row r="10" spans="2:10" ht="16.5" customHeight="1">
+      <c r="B10" s="20"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="2">
+        <v>0.51321695605838002</v>
+      </c>
+      <c r="E10" s="16">
+        <v>0.53102199794728799</v>
+      </c>
+      <c r="F10" s="12">
+        <v>0.531515353985204</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" ht="15">
+      <c r="B11" s="21"/>
+      <c r="C11" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="D10" s="9">
-        <v>0.51321695605838002</v>
-      </c>
-      <c r="E10" s="23">
-        <v>0.53102199794728799</v>
-      </c>
-      <c r="F10" s="19">
-        <v>0.531515353985204</v>
-      </c>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B11" s="27"/>
-      <c r="C11" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="D11" s="11">
+      <c r="D11" s="4">
         <f>D10-D9</f>
         <v>-3.4102014273450942E-2</v>
       </c>
-      <c r="E11" s="24">
+      <c r="E11" s="17">
         <f>E10-E9</f>
         <v>1.9099740110537944E-2</v>
       </c>
-      <c r="F11" s="20">
+      <c r="F11" s="13">
         <f>F10-F9</f>
         <v>-4.3141248933949994E-2</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B12" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="D12" s="9">
+    <row r="12" spans="2:10">
+      <c r="B12" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" s="6"/>
+      <c r="D12" s="2">
         <v>1.8043290933586101E-2</v>
       </c>
-      <c r="E12" s="23">
+      <c r="E12" s="16">
         <v>1.4592593089977599E-2</v>
       </c>
-      <c r="F12" s="19">
+      <c r="F12" s="12">
         <v>7.0661052539501999E-3</v>
       </c>
       <c r="H12" t="b">
@@ -2145,68 +4138,62 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B13" s="26"/>
-      <c r="C13" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="D13" s="22">
+    <row r="13" spans="2:10">
+      <c r="B13" s="20"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="15">
         <v>0.98847374363714202</v>
       </c>
-      <c r="E13" s="23">
+      <c r="E13" s="16">
         <v>0.98275893932599301</v>
       </c>
-      <c r="F13" s="19">
+      <c r="F13" s="12">
         <v>0.98888395208439495</v>
       </c>
     </row>
-    <row r="14" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="26"/>
-      <c r="C14" s="13" t="s">
+    <row r="14" spans="2:10" ht="16.5" customHeight="1">
+      <c r="B14" s="20"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="2">
+        <v>0.976338380896693</v>
+      </c>
+      <c r="E14" s="16">
+        <v>0.94856851807495501</v>
+      </c>
+      <c r="F14" s="12">
+        <v>0.98182697373651096</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" ht="15">
+      <c r="B15" s="21"/>
+      <c r="C15" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="D14" s="9">
-        <v>0.976338380896693</v>
-      </c>
-      <c r="E14" s="23">
-        <v>0.94856851807495501</v>
-      </c>
-      <c r="F14" s="19">
-        <v>0.98182697373651096</v>
-      </c>
-    </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B15" s="27"/>
-      <c r="C15" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="D15" s="11">
+      <c r="D15" s="4">
         <f>D14-D13</f>
         <v>-1.2135362740449018E-2</v>
       </c>
-      <c r="E15" s="24">
+      <c r="E15" s="17">
         <f>E14-E13</f>
         <v>-3.4190421251037995E-2</v>
       </c>
-      <c r="F15" s="20">
+      <c r="F15" s="13">
         <f>F14-F13</f>
         <v>-7.0569783478839909E-3</v>
       </c>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B16" s="25" t="s">
-        <v>48</v>
-      </c>
-      <c r="C16" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="D16" s="9">
+    <row r="16" spans="2:10">
+      <c r="B16" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="6"/>
+      <c r="D16" s="2">
         <v>3.7487329238110503E-2</v>
       </c>
-      <c r="E16" s="23">
+      <c r="E16" s="16">
         <v>3.78571134410128E-2</v>
       </c>
-      <c r="F16" s="19">
+      <c r="F16" s="12">
         <v>1.23113100057045E-2</v>
       </c>
       <c r="H16" t="b">
@@ -2222,68 +4209,62 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B17" s="26"/>
-      <c r="C17" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="D17" s="22">
+    <row r="17" spans="2:10">
+      <c r="B17" s="20"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="15">
         <v>0.65795852996008097</v>
       </c>
-      <c r="E17" s="23">
+      <c r="E17" s="16">
         <v>0.66725667618805895</v>
       </c>
-      <c r="F17" s="19">
+      <c r="F17" s="12">
         <v>0.69867159092716702</v>
       </c>
     </row>
-    <row r="18" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="26"/>
-      <c r="C18" s="13" t="s">
+    <row r="18" spans="2:10" ht="16.5" customHeight="1">
+      <c r="B18" s="20"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="2">
+        <v>0.61793481809617501</v>
+      </c>
+      <c r="E18" s="16">
+        <v>0.62241699122894401</v>
+      </c>
+      <c r="F18" s="12">
+        <v>0.630522827712378</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" ht="15">
+      <c r="B19" s="21"/>
+      <c r="C19" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="D18" s="9">
-        <v>0.61793481809617501</v>
-      </c>
-      <c r="E18" s="23">
-        <v>0.62241699122894401</v>
-      </c>
-      <c r="F18" s="19">
-        <v>0.630522827712378</v>
-      </c>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B19" s="27"/>
-      <c r="C19" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="D19" s="11">
+      <c r="D19" s="4">
         <f>D18-D17</f>
         <v>-4.0023711863905964E-2</v>
       </c>
-      <c r="E19" s="24">
+      <c r="E19" s="17">
         <f>E18-E17</f>
         <v>-4.4839684959114945E-2</v>
       </c>
-      <c r="F19" s="20">
+      <c r="F19" s="13">
         <f>F18-F17</f>
         <v>-6.8148763214789021E-2</v>
       </c>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B20" s="25" t="s">
-        <v>49</v>
-      </c>
-      <c r="C20" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="D20" s="9">
+    <row r="20" spans="2:10">
+      <c r="B20" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" s="6"/>
+      <c r="D20" s="2">
         <v>2.2365497027515901E-2</v>
       </c>
-      <c r="E20" s="23">
+      <c r="E20" s="16">
         <v>2.4671099397125199E-2</v>
       </c>
-      <c r="F20" s="19">
+      <c r="F20" s="12">
         <v>1.0578861156285899E-2</v>
       </c>
       <c r="H20" t="b">
@@ -2299,68 +4280,62 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B21" s="26"/>
-      <c r="C21" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="D21" s="22">
+    <row r="21" spans="2:10">
+      <c r="B21" s="20"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="15">
         <v>0.47786140240302599</v>
       </c>
-      <c r="E21" s="23">
+      <c r="E21" s="16">
         <v>0.43697895740280102</v>
       </c>
-      <c r="F21" s="19">
+      <c r="F21" s="12">
         <v>0.53249315802663499</v>
       </c>
     </row>
-    <row r="22" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="26"/>
-      <c r="C22" s="13" t="s">
+    <row r="22" spans="2:10" ht="16.5" customHeight="1">
+      <c r="B22" s="20"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="2">
+        <v>0.45384412596574503</v>
+      </c>
+      <c r="E22" s="16">
+        <v>0.46533683967913803</v>
+      </c>
+      <c r="F22" s="12">
+        <v>0.45973744390136001</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" ht="15">
+      <c r="B23" s="21"/>
+      <c r="C23" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="D22" s="9">
-        <v>0.45384412596574503</v>
-      </c>
-      <c r="E22" s="23">
-        <v>0.46533683967913803</v>
-      </c>
-      <c r="F22" s="19">
-        <v>0.45973744390136001</v>
-      </c>
-    </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B23" s="27"/>
-      <c r="C23" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="D23" s="11">
+      <c r="D23" s="4">
         <f>D22-D21</f>
         <v>-2.4017276437280966E-2</v>
       </c>
-      <c r="E23" s="24">
+      <c r="E23" s="17">
         <f>E22-E21</f>
         <v>2.835788227633701E-2</v>
       </c>
-      <c r="F23" s="20">
+      <c r="F23" s="13">
         <f>F22-F21</f>
         <v>-7.2755714125274984E-2</v>
       </c>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B24" s="25" t="s">
-        <v>50</v>
-      </c>
-      <c r="C24" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="D24" s="9">
+    <row r="24" spans="2:10">
+      <c r="B24" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" s="6"/>
+      <c r="D24" s="2">
         <v>2.2502290559711501E-2</v>
       </c>
-      <c r="E24" s="23">
+      <c r="E24" s="16">
         <v>3.7779284936843398E-2</v>
       </c>
-      <c r="F24" s="19">
+      <c r="F24" s="12">
         <v>2.4761188831014E-3</v>
       </c>
       <c r="H24" t="b">
@@ -2376,68 +4351,62 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B25" s="26"/>
-      <c r="C25" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="D25" s="22">
+    <row r="25" spans="2:10">
+      <c r="B25" s="20"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="15">
         <v>0.54877303871056204</v>
       </c>
-      <c r="E25" s="23">
+      <c r="E25" s="16">
         <v>0.45973371060712498</v>
       </c>
-      <c r="F25" s="19">
+      <c r="F25" s="12">
         <v>0.58704627840722501</v>
       </c>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B26" s="26"/>
-      <c r="C26" s="13" t="s">
+    <row r="26" spans="2:10">
+      <c r="B26" s="20"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="2">
+        <v>0.56261075900048596</v>
+      </c>
+      <c r="E26" s="16">
+        <v>0.40569581778109898</v>
+      </c>
+      <c r="F26" s="12">
+        <v>0.57262384483879103</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10" ht="15">
+      <c r="B27" s="21"/>
+      <c r="C27" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="D26" s="9">
-        <v>0.56261075900048596</v>
-      </c>
-      <c r="E26" s="23">
-        <v>0.40569581778109898</v>
-      </c>
-      <c r="F26" s="19">
-        <v>0.57262384483879103</v>
-      </c>
-    </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B27" s="27"/>
-      <c r="C27" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="D27" s="11">
+      <c r="D27" s="4">
         <f>D26-D25</f>
         <v>1.3837720289923916E-2</v>
       </c>
-      <c r="E27" s="24">
+      <c r="E27" s="17">
         <f>E26-E25</f>
         <v>-5.4037892826026002E-2</v>
       </c>
-      <c r="F27" s="20">
+      <c r="F27" s="13">
         <f>F26-F25</f>
         <v>-1.4422433568433979E-2</v>
       </c>
     </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B28" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="C28" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="D28" s="9">
+    <row r="28" spans="2:10">
+      <c r="B28" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="C28" s="6"/>
+      <c r="D28" s="2">
         <v>2.5093379297579901E-2</v>
       </c>
-      <c r="E28" s="23">
+      <c r="E28" s="16">
         <v>1.6191324233012699E-2</v>
       </c>
-      <c r="F28" s="19">
+      <c r="F28" s="12">
         <v>3.6273493619296002E-3</v>
       </c>
       <c r="H28" t="b">
@@ -2453,50 +4422,46 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B29" s="26"/>
-      <c r="C29" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="D29" s="22">
+    <row r="29" spans="2:10">
+      <c r="B29" s="20"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="15">
         <v>0.55812760815291595</v>
       </c>
-      <c r="E29" s="23">
+      <c r="E29" s="16">
         <v>0.55920433648563295</v>
       </c>
-      <c r="F29" s="19">
+      <c r="F29" s="12">
         <v>0.58304667288122403</v>
       </c>
     </row>
-    <row r="30" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="26"/>
-      <c r="C30" s="13" t="s">
+    <row r="30" spans="2:10" ht="16.5" customHeight="1">
+      <c r="B30" s="20"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="2">
+        <v>0.51996660857136801</v>
+      </c>
+      <c r="E30" s="16">
+        <v>0.50123255471193495</v>
+      </c>
+      <c r="F30" s="12">
+        <v>0.53069962353919298</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10" ht="15">
+      <c r="B31" s="21"/>
+      <c r="C31" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="D30" s="9">
-        <v>0.51996660857136801</v>
-      </c>
-      <c r="E30" s="23">
-        <v>0.50123255471193495</v>
-      </c>
-      <c r="F30" s="19">
-        <v>0.53069962353919298</v>
-      </c>
-    </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B31" s="27"/>
-      <c r="C31" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="D31" s="11">
+      <c r="D31" s="4">
         <f>D30-D29</f>
         <v>-3.816099958154795E-2</v>
       </c>
-      <c r="E31" s="24">
+      <c r="E31" s="17">
         <f>E30-E29</f>
         <v>-5.7971781773697995E-2</v>
       </c>
-      <c r="F31" s="20">
+      <c r="F31" s="13">
         <f>F30-F29</f>
         <v>-5.2347049342031049E-2</v>
       </c>
@@ -2535,7 +4500,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="96" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="89" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <colBreaks count="1" manualBreakCount="1">
     <brk id="7" max="31" man="1"/>
   </colBreaks>

</xml_diff>